<commit_message>
issue with Simple Template address #196
</commit_message>
<xml_diff>
--- a/tests/Templates/Simple.xlsx
+++ b/tests/Templates/Simple.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ЭтаКнига"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sources\asr\ClosedXML.Report\tests\Templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="600" yWindow="615" windowWidth="17400" windowHeight="11460"/>
   </bookViews>
@@ -70,14 +75,14 @@
     <t>{{Contact}}</t>
   </si>
   <si>
-    <t>&amp;={{Addr1}}&amp;" "&amp;{{Addr2}}</t>
+    <t>&amp;="{{Addr1}}"&amp;" "&amp;"{{Addr2}}"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
       <name val="Arial"/>
@@ -402,6 +407,14 @@
       <color rgb="FF9F7CFF"/>
     </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -795,15 +808,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Лист1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.6640625" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
@@ -818,7 +833,7 @@
     <col min="12" max="12" width="4.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="51" customHeight="1">
+    <row r="1" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="27" t="s">
         <v>9</v>
@@ -834,7 +849,7 @@
       <c r="K1" s="28"/>
       <c r="L1" s="28"/>
     </row>
-    <row r="2" spans="1:12" ht="12.75">
+    <row r="2" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -848,7 +863,7 @@
       <c r="K2" s="5"/>
       <c r="L2" s="4"/>
     </row>
-    <row r="3" spans="1:12" ht="18">
+    <row r="3" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="8"/>
       <c r="B3" s="9" t="s">
         <v>8</v>
@@ -866,7 +881,7 @@
       <c r="K3" s="17"/>
       <c r="L3" s="18"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="10"/>
       <c r="C4" s="6"/>
@@ -880,13 +895,13 @@
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="12">
+    <row r="6" spans="1:12" ht="12" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="30" t="s">
         <v>18</v>
@@ -902,7 +917,7 @@
       <c r="K6" s="15"/>
       <c r="L6" s="16"/>
     </row>
-    <row r="7" spans="1:12" ht="12">
+    <row r="7" spans="1:12" ht="12" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="34"/>
       <c r="C7" s="3"/>
@@ -916,7 +931,7 @@
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="9" t="s">
         <v>1</v>
@@ -931,7 +946,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="12">
+    <row r="9" spans="1:12" ht="12" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="31" t="s">
         <v>10</v>
@@ -953,7 +968,7 @@
       </c>
       <c r="L9" s="19"/>
     </row>
-    <row r="10" spans="1:12" ht="12">
+    <row r="10" spans="1:12" ht="12" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="1"/>
       <c r="C10" s="7"/>
@@ -967,7 +982,7 @@
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="9" t="s">
         <v>4</v>
@@ -979,7 +994,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="12">
+    <row r="12" spans="1:12" ht="12" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="32" t="s">
         <v>15</v>
@@ -999,13 +1014,13 @@
       <c r="K12" s="12"/>
       <c r="L12" s="22"/>
     </row>
-    <row r="14" spans="1:12" ht="12">
+    <row r="14" spans="1:12" ht="12" x14ac:dyDescent="0.2">
       <c r="B14" s="33"/>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B15" s="29"/>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B16" s="29"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
issue with Simple Template address #196 (#238)
</commit_message>
<xml_diff>
--- a/tests/Templates/Simple.xlsx
+++ b/tests/Templates/Simple.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ЭтаКнига"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sources\asr\ClosedXML.Report\tests\Templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="600" yWindow="615" windowWidth="17400" windowHeight="11460"/>
   </bookViews>
@@ -70,14 +75,14 @@
     <t>{{Contact}}</t>
   </si>
   <si>
-    <t>&amp;={{Addr1}}&amp;" "&amp;{{Addr2}}</t>
+    <t>&amp;="{{Addr1}}"&amp;" "&amp;"{{Addr2}}"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
       <name val="Arial"/>
@@ -402,6 +407,14 @@
       <color rgb="FF9F7CFF"/>
     </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -795,15 +808,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Лист1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.6640625" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
@@ -818,7 +833,7 @@
     <col min="12" max="12" width="4.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="51" customHeight="1">
+    <row r="1" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="27" t="s">
         <v>9</v>
@@ -834,7 +849,7 @@
       <c r="K1" s="28"/>
       <c r="L1" s="28"/>
     </row>
-    <row r="2" spans="1:12" ht="12.75">
+    <row r="2" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -848,7 +863,7 @@
       <c r="K2" s="5"/>
       <c r="L2" s="4"/>
     </row>
-    <row r="3" spans="1:12" ht="18">
+    <row r="3" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="8"/>
       <c r="B3" s="9" t="s">
         <v>8</v>
@@ -866,7 +881,7 @@
       <c r="K3" s="17"/>
       <c r="L3" s="18"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="10"/>
       <c r="C4" s="6"/>
@@ -880,13 +895,13 @@
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="12">
+    <row r="6" spans="1:12" ht="12" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="30" t="s">
         <v>18</v>
@@ -902,7 +917,7 @@
       <c r="K6" s="15"/>
       <c r="L6" s="16"/>
     </row>
-    <row r="7" spans="1:12" ht="12">
+    <row r="7" spans="1:12" ht="12" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="34"/>
       <c r="C7" s="3"/>
@@ -916,7 +931,7 @@
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="9" t="s">
         <v>1</v>
@@ -931,7 +946,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="12">
+    <row r="9" spans="1:12" ht="12" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="31" t="s">
         <v>10</v>
@@ -953,7 +968,7 @@
       </c>
       <c r="L9" s="19"/>
     </row>
-    <row r="10" spans="1:12" ht="12">
+    <row r="10" spans="1:12" ht="12" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="1"/>
       <c r="C10" s="7"/>
@@ -967,7 +982,7 @@
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="9" t="s">
         <v>4</v>
@@ -979,7 +994,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="12">
+    <row r="12" spans="1:12" ht="12" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="32" t="s">
         <v>15</v>
@@ -999,13 +1014,13 @@
       <c r="K12" s="12"/>
       <c r="L12" s="22"/>
     </row>
-    <row r="14" spans="1:12" ht="12">
+    <row r="14" spans="1:12" ht="12" x14ac:dyDescent="0.2">
       <c r="B14" s="33"/>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B15" s="29"/>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B16" s="29"/>
     </row>
   </sheetData>

</xml_diff>